<commit_message>
parameter adjustment. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/20150522--compare.xlsx
+++ b/INRC2_Simulator/log/20150522--compare.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="61290" yWindow="0" windowWidth="23580" windowHeight="12570"/>
+    <workbookView xWindow="62460" yWindow="0" windowWidth="23580" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="201504200152--Win8.1--GreedyIni" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>TSR</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -83,20 +83,16 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>ACBR_iBNO</t>
+  </si>
+  <si>
+    <t>TSR_RMIE</t>
+  </si>
+  <si>
     <t>1;w1,w1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR_iBNO</t>
-  </si>
-  <si>
-    <t>TSR_RMIE</t>
-  </si>
-  <si>
-    <t>1;w1,w1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>BTS</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -138,6 +134,18 @@
   </si>
   <si>
     <t>1;0,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5;0,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR_BNO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;w1,w1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -921,7 +929,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -995,6 +1003,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1384,7 +1395,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R10" sqref="R10"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1396,33 +1407,35 @@
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30"/>
+        <v>21</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>16</v>
@@ -1437,32 +1450,34 @@
         <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="27"/>
+        <v>26</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="28"/>
     </row>
     <row r="3" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>18</v>
@@ -1471,34 +1486,36 @@
         <v>18</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="27"/>
+        <v>30</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -1530,7 +1547,7 @@
       </c>
       <c r="H4" s="12">
         <f t="shared" si="0"/>
-        <v>3983.9067857142863</v>
+        <v>3864.9107142857142</v>
       </c>
       <c r="I4" s="12">
         <f t="shared" si="0"/>
@@ -1550,7 +1567,7 @@
       </c>
       <c r="M4" s="14">
         <f t="shared" si="0"/>
-        <v>3969.9782142857143</v>
+        <v>3867.3660714285716</v>
       </c>
       <c r="N4" s="21"/>
     </row>
@@ -1584,7 +1601,7 @@
       </c>
       <c r="H5" s="11">
         <f t="shared" si="1"/>
-        <v>3880.6700000000005</v>
+        <v>3809.7321428571427</v>
       </c>
       <c r="I5" s="11">
         <f t="shared" si="1"/>
@@ -1604,10 +1621,10 @@
       </c>
       <c r="M5" s="15">
         <f t="shared" si="1"/>
-        <v>3896.6521428571432</v>
+        <v>3798.3928571428573</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
@@ -1633,7 +1650,7 @@
         <v>5303.75</v>
       </c>
       <c r="H6" s="7">
-        <v>5213.75</v>
+        <v>5378.75</v>
       </c>
       <c r="I6" s="1">
         <v>5445</v>
@@ -1648,7 +1665,7 @@
         <v>5320.63</v>
       </c>
       <c r="M6" s="2">
-        <v>5401.88</v>
+        <v>5302.5</v>
       </c>
       <c r="N6" s="23" t="s">
         <v>2</v>
@@ -1677,7 +1694,7 @@
         <v>5118.13</v>
       </c>
       <c r="H7" s="7">
-        <v>5040.63</v>
+        <v>4642.5</v>
       </c>
       <c r="I7" s="1">
         <v>4530</v>
@@ -1692,7 +1709,7 @@
         <v>4636.25</v>
       </c>
       <c r="M7" s="2">
-        <v>4845</v>
+        <v>4661.25</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>3</v>
@@ -1721,7 +1738,7 @@
         <v>3434.38</v>
       </c>
       <c r="H8" s="7">
-        <v>3301.25</v>
+        <v>3278.75</v>
       </c>
       <c r="I8" s="1">
         <v>3403.75</v>
@@ -1736,7 +1753,7 @@
         <v>3258.75</v>
       </c>
       <c r="M8" s="2">
-        <v>3311.25</v>
+        <v>3200</v>
       </c>
       <c r="N8" s="23" t="s">
         <v>4</v>
@@ -1765,7 +1782,7 @@
         <v>6051.25</v>
       </c>
       <c r="H9" s="7">
-        <v>5937.5</v>
+        <v>5795</v>
       </c>
       <c r="I9" s="1">
         <v>5955</v>
@@ -1780,7 +1797,7 @@
         <v>5832.5</v>
       </c>
       <c r="M9" s="2">
-        <v>5875</v>
+        <v>5890</v>
       </c>
       <c r="N9" s="23" t="s">
         <v>5</v>
@@ -1809,7 +1826,7 @@
         <v>2306.25</v>
       </c>
       <c r="H10" s="7">
-        <v>2267.5</v>
+        <v>2167.5</v>
       </c>
       <c r="I10" s="1">
         <v>2237.5</v>
@@ -1824,7 +1841,7 @@
         <v>2208.75</v>
       </c>
       <c r="M10" s="2">
-        <v>2338.75</v>
+        <v>2240</v>
       </c>
       <c r="N10" s="23" t="s">
         <v>6</v>
@@ -1853,7 +1870,7 @@
         <v>4120</v>
       </c>
       <c r="H11" s="7">
-        <v>4220</v>
+        <v>4088.75</v>
       </c>
       <c r="I11" s="1">
         <v>4128.75</v>
@@ -1868,7 +1885,7 @@
         <v>4108.75</v>
       </c>
       <c r="M11" s="2">
-        <v>4173.75</v>
+        <v>4003.75</v>
       </c>
       <c r="N11" s="23" t="s">
         <v>7</v>
@@ -1897,7 +1914,7 @@
         <v>4396.25</v>
       </c>
       <c r="H12" s="7">
-        <v>4392.5</v>
+        <v>4242.5</v>
       </c>
       <c r="I12" s="1">
         <v>4317.5</v>
@@ -1912,7 +1929,7 @@
         <v>4300</v>
       </c>
       <c r="M12" s="2">
-        <v>4386.25</v>
+        <v>4237.5</v>
       </c>
       <c r="N12" s="23" t="s">
         <v>8</v>
@@ -1941,7 +1958,7 @@
         <v>7261.25</v>
       </c>
       <c r="H13" s="7">
-        <v>7071.25</v>
+        <v>7210</v>
       </c>
       <c r="I13" s="1">
         <v>7110</v>
@@ -1956,7 +1973,7 @@
         <v>7060</v>
       </c>
       <c r="M13" s="2">
-        <v>7400</v>
+        <v>7107.5</v>
       </c>
       <c r="N13" s="23" t="s">
         <v>9</v>
@@ -1985,7 +2002,7 @@
         <v>3252.5</v>
       </c>
       <c r="H14" s="7">
-        <v>3281.25</v>
+        <v>3240</v>
       </c>
       <c r="I14" s="1">
         <v>3181.25</v>
@@ -2000,7 +2017,7 @@
         <v>3197.5</v>
       </c>
       <c r="M14" s="2">
-        <v>3250</v>
+        <v>3212.5</v>
       </c>
       <c r="N14" s="23" t="s">
         <v>10</v>
@@ -2029,7 +2046,7 @@
         <v>4328.75</v>
       </c>
       <c r="H15" s="7">
-        <v>4340</v>
+        <v>4092.5</v>
       </c>
       <c r="I15" s="1">
         <v>4231.25</v>
@@ -2044,7 +2061,7 @@
         <v>4083.75</v>
       </c>
       <c r="M15" s="2">
-        <v>4252.5</v>
+        <v>4177.5</v>
       </c>
       <c r="N15" s="23" t="s">
         <v>11</v>
@@ -2073,7 +2090,7 @@
         <v>1931.25</v>
       </c>
       <c r="H16" s="7">
-        <v>1871.25</v>
+        <v>1882.5</v>
       </c>
       <c r="I16" s="1">
         <v>1908.75</v>
@@ -2088,7 +2105,7 @@
         <v>1916.25</v>
       </c>
       <c r="M16" s="2">
-        <v>1955</v>
+        <v>1906.25</v>
       </c>
       <c r="N16" s="23" t="s">
         <v>12</v>
@@ -2117,7 +2134,7 @@
         <v>3225</v>
       </c>
       <c r="H17" s="7">
-        <v>3290</v>
+        <v>3125</v>
       </c>
       <c r="I17" s="1">
         <v>3161.25</v>
@@ -2132,7 +2149,7 @@
         <v>3290</v>
       </c>
       <c r="M17" s="2">
-        <v>3233.75</v>
+        <v>3126.25</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>13</v>
@@ -2161,7 +2178,7 @@
         <v>2032.5</v>
       </c>
       <c r="H18" s="7">
-        <v>2031.25</v>
+        <v>2046.25</v>
       </c>
       <c r="I18" s="1">
         <v>2051.25</v>
@@ -2176,7 +2193,7 @@
         <v>2031.25</v>
       </c>
       <c r="M18" s="2">
-        <v>2025</v>
+        <v>2002.5</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>14</v>
@@ -2205,7 +2222,7 @@
         <v>2127.5</v>
       </c>
       <c r="H19" s="7">
-        <v>2071.25</v>
+        <v>2146.25</v>
       </c>
       <c r="I19" s="1">
         <v>2137.5</v>
@@ -2220,7 +2237,7 @@
         <v>2128.75</v>
       </c>
       <c r="M19" s="2">
-        <v>2105</v>
+        <v>2110</v>
       </c>
       <c r="N19" s="23" t="s">
         <v>15</v>
@@ -2256,7 +2273,7 @@
       </c>
       <c r="H20" s="8">
         <f t="shared" si="2"/>
-        <v>4087.1435714285717</v>
+        <v>3920.0892857142858</v>
       </c>
       <c r="I20" s="8">
         <f t="shared" si="2"/>
@@ -2276,10 +2293,10 @@
       </c>
       <c r="M20" s="9">
         <f t="shared" si="2"/>
-        <v>4043.3042857142859</v>
+        <v>3936.3392857142858</v>
       </c>
       <c r="N20" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
@@ -2305,7 +2322,7 @@
         <v>5895.63</v>
       </c>
       <c r="H21" s="7">
-        <v>5820</v>
+        <v>5568.75</v>
       </c>
       <c r="I21" s="7">
         <v>5692.5</v>
@@ -2320,7 +2337,7 @@
         <v>5812.5</v>
       </c>
       <c r="M21" s="7">
-        <v>5829.38</v>
+        <v>5663.75</v>
       </c>
       <c r="N21" s="23" t="s">
         <v>2</v>
@@ -2349,7 +2366,7 @@
         <v>5493.13</v>
       </c>
       <c r="H22" s="7">
-        <v>5466.25</v>
+        <v>4822.5</v>
       </c>
       <c r="I22" s="7">
         <v>4838.75</v>
@@ -2364,7 +2381,7 @@
         <v>5013.75</v>
       </c>
       <c r="M22" s="7">
-        <v>5094.38</v>
+        <v>5031.25</v>
       </c>
       <c r="N22" s="23" t="s">
         <v>3</v>
@@ -2393,7 +2410,7 @@
         <v>3375</v>
       </c>
       <c r="H23" s="7">
-        <v>3345</v>
+        <v>3342.5</v>
       </c>
       <c r="I23" s="7">
         <v>3307.5</v>
@@ -2408,7 +2425,7 @@
         <v>3276.88</v>
       </c>
       <c r="M23" s="7">
-        <v>3486.25</v>
+        <v>3387.5</v>
       </c>
       <c r="N23" s="23" t="s">
         <v>4</v>
@@ -2437,7 +2454,7 @@
         <v>6596.88</v>
       </c>
       <c r="H24" s="7">
-        <v>6549.38</v>
+        <v>6310</v>
       </c>
       <c r="I24" s="7">
         <v>6273.75</v>
@@ -2452,7 +2469,7 @@
         <v>6241.25</v>
       </c>
       <c r="M24" s="7">
-        <v>6435</v>
+        <v>6316.25</v>
       </c>
       <c r="N24" s="23" t="s">
         <v>5</v>
@@ -2481,7 +2498,7 @@
         <v>3101.88</v>
       </c>
       <c r="H25" s="7">
-        <v>2940.63</v>
+        <v>2727.5</v>
       </c>
       <c r="I25" s="7">
         <v>2673.75</v>
@@ -2496,7 +2513,7 @@
         <v>2613.75</v>
       </c>
       <c r="M25" s="7">
-        <v>2842.5</v>
+        <v>2652.5</v>
       </c>
       <c r="N25" s="23" t="s">
         <v>6</v>
@@ -2525,7 +2542,7 @@
         <v>5095</v>
       </c>
       <c r="H26" s="7">
-        <v>5007.5</v>
+        <v>4661.25</v>
       </c>
       <c r="I26" s="7">
         <v>4611.25</v>
@@ -2540,7 +2557,7 @@
         <v>4753.75</v>
       </c>
       <c r="M26" s="7">
-        <v>4891.25</v>
+        <v>4606.25</v>
       </c>
       <c r="N26" s="23" t="s">
         <v>7</v>
@@ -2569,7 +2586,7 @@
         <v>4252.5</v>
       </c>
       <c r="H27" s="7">
-        <v>4176.25</v>
+        <v>4122.5</v>
       </c>
       <c r="I27" s="7">
         <v>4277.5</v>
@@ -2584,7 +2601,7 @@
         <v>4265</v>
       </c>
       <c r="M27" s="7">
-        <v>4182.5</v>
+        <v>4217.5</v>
       </c>
       <c r="N27" s="23" t="s">
         <v>8</v>
@@ -2613,7 +2630,7 @@
         <v>7091.25</v>
       </c>
       <c r="H28" s="7">
-        <v>7072.5</v>
+        <v>6861.25</v>
       </c>
       <c r="I28" s="7">
         <v>6921.25</v>
@@ -2628,7 +2645,7 @@
         <v>6853.75</v>
       </c>
       <c r="M28" s="7">
-        <v>7100</v>
+        <v>6857.5</v>
       </c>
       <c r="N28" s="23" t="s">
         <v>9</v>
@@ -2657,7 +2674,7 @@
         <v>3582.5</v>
       </c>
       <c r="H29" s="7">
-        <v>3480</v>
+        <v>3507.5</v>
       </c>
       <c r="I29" s="7">
         <v>3515</v>
@@ -2672,7 +2689,7 @@
         <v>3342.5</v>
       </c>
       <c r="M29" s="7">
-        <v>3522.5</v>
+        <v>3401.25</v>
       </c>
       <c r="N29" s="23" t="s">
         <v>10</v>
@@ -2701,7 +2718,7 @@
         <v>4002.5</v>
       </c>
       <c r="H30" s="7">
-        <v>3988.75</v>
+        <v>3832.5</v>
       </c>
       <c r="I30" s="7">
         <v>3812.5</v>
@@ -2716,7 +2733,7 @@
         <v>3731.25</v>
       </c>
       <c r="M30" s="7">
-        <v>3971.25</v>
+        <v>3803.75</v>
       </c>
       <c r="N30" s="23" t="s">
         <v>11</v>
@@ -2745,7 +2762,7 @@
         <v>1982.5</v>
       </c>
       <c r="H31" s="7">
-        <v>2010</v>
+        <v>1996.25</v>
       </c>
       <c r="I31" s="7">
         <v>1873.75</v>
@@ -2760,7 +2777,7 @@
         <v>1946.25</v>
       </c>
       <c r="M31" s="7">
-        <v>1953.75</v>
+        <v>1942.5</v>
       </c>
       <c r="N31" s="23" t="s">
         <v>12</v>
@@ -2789,7 +2806,7 @@
         <v>2703.75</v>
       </c>
       <c r="H32" s="7">
-        <v>2825</v>
+        <v>2763.75</v>
       </c>
       <c r="I32" s="7">
         <v>2726.25</v>
@@ -2804,7 +2821,7 @@
         <v>2785</v>
       </c>
       <c r="M32" s="7">
-        <v>2762.5</v>
+        <v>2701.25</v>
       </c>
       <c r="N32" s="23" t="s">
         <v>13</v>
@@ -2833,7 +2850,7 @@
         <v>2261.25</v>
       </c>
       <c r="H33" s="7">
-        <v>2247.5</v>
+        <v>2163.75</v>
       </c>
       <c r="I33" s="7">
         <v>2192.5</v>
@@ -2848,7 +2865,7 @@
         <v>2201.25</v>
       </c>
       <c r="M33" s="7">
-        <v>2248.75</v>
+        <v>2218.75</v>
       </c>
       <c r="N33" s="23" t="s">
         <v>14</v>
@@ -2877,7 +2894,7 @@
         <v>2235</v>
       </c>
       <c r="H34" s="13">
-        <v>2291.25</v>
+        <v>2201.25</v>
       </c>
       <c r="I34" s="13">
         <v>2263.75</v>
@@ -2892,7 +2909,7 @@
         <v>2266.25</v>
       </c>
       <c r="M34" s="13">
-        <v>2286.25</v>
+        <v>2308.75</v>
       </c>
       <c r="N34" s="18" t="s">
         <v>15</v>

</xml_diff>